<commit_message>
Insertadas evidencias en las horas computadas
</commit_message>
<xml_diff>
--- a/Horas computadas/Horas - Comité de Finanzas - Grupo 1.xlsx
+++ b/Horas computadas/Horas - Comité de Finanzas - Grupo 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7650" windowWidth="28800" windowHeight="12795" tabRatio="364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8100" windowWidth="28800" windowHeight="12795" tabRatio="364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
   <si>
     <t>Grupo</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Horas (totales)</t>
-  </si>
-  <si>
     <t>Comité</t>
   </si>
   <si>
@@ -128,10 +125,19 @@
     <t>Evidencia 16</t>
   </si>
   <si>
-    <t>Jornadas 06/11/17</t>
-  </si>
-  <si>
-    <t>Jornadas 09/11/17</t>
+    <t>Horas (trabajo)</t>
+  </si>
+  <si>
+    <t>Horas (jornadas)</t>
+  </si>
+  <si>
+    <t>Horas(totales)</t>
+  </si>
+  <si>
+    <t>Jornadas 06/11</t>
+  </si>
+  <si>
+    <t>Jornadas 09/11</t>
   </si>
 </sst>
 </file>
@@ -141,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +192,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +239,20 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -243,35 +269,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="7" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Énfasis4" xfId="2" builtinId="41"/>
     <cellStyle name="Énfasis5" xfId="3" builtinId="45"/>
     <cellStyle name="Énfasis6" xfId="4" builtinId="49"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 3" xfId="1" builtinId="18"/>
   </cellStyles>
@@ -590,355 +750,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="7"/>
-    <col min="2" max="2" width="20.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="7" customWidth="1"/>
-    <col min="8" max="22" width="11.42578125" style="7"/>
-    <col min="23" max="23" width="17.28515625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" style="7" customWidth="1"/>
-    <col min="25" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
+    <col min="11" max="22" width="11.42578125" style="1"/>
+    <col min="23" max="23" width="12.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+    </row>
+    <row r="2" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="I2" s="9">
+        <f>SUM(G2,H2)</f>
+        <v>0.77569444444444446</v>
+      </c>
+      <c r="J2" s="11">
+        <f>SUM(F2,I2)</f>
+        <v>1.7027777777777779</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+    </row>
+    <row r="3" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="B3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1.070138888888889</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="38">
+        <f t="shared" ref="I3:I5" si="0">SUM(G3,H3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" ref="J3:J5" si="1">SUM(F3,I3)</f>
+        <v>1.070138888888889</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="L3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="M3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="N3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="Q3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="R3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="S3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="T3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="U3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="W3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="X3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="Y3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="Z3" s="30"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="4" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J4" s="11">
+        <f t="shared" si="1"/>
+        <v>1.2083333333333333</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="14">
-        <f>SUM(G2:X2)</f>
-        <v>1.7027777777777777</v>
-      </c>
-      <c r="G2" s="9">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H2" s="9">
-        <v>6.5972222222222224E-2</v>
-      </c>
-      <c r="I2" s="9">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="J2" s="9">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="K2" s="9">
-        <v>6.25E-2</v>
-      </c>
-      <c r="L2" s="9">
-        <v>6.5972222222222224E-2</v>
-      </c>
-      <c r="M2" s="9">
-        <v>6.5972222222222224E-2</v>
-      </c>
-      <c r="N2" s="9">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="O2" s="9">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="P2" s="9">
-        <v>3.125E-2</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>5.9027777777777783E-2</v>
-      </c>
-      <c r="R2" s="9">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="S2" s="9">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="T2" s="9">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="U2" s="9">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="V2" s="10">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="W2" s="9">
-        <v>0.39374999999999999</v>
-      </c>
-      <c r="X2" s="9">
-        <v>0.38194444444444442</v>
-      </c>
+      <c r="E5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="37">
+        <v>0.3125</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="34">
+        <f t="shared" si="1"/>
+        <v>0.3125</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="36"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="13">
-        <f>SUM(G3:U3)</f>
-        <v>1.0701388888888888</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="H3" s="9">
-        <v>9.375E-2</v>
-      </c>
-      <c r="I3" s="9">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="J3" s="9">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="K3" s="9">
-        <v>8.6805555555555566E-2</v>
-      </c>
-      <c r="L3" s="9">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="M3" s="9">
-        <v>9.375E-2</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0.10486111111111111</v>
-      </c>
-      <c r="O3" s="10">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P3" s="9">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="R3" s="9">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="S3" s="9">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="T3" s="9">
-        <v>0.38194444444444442</v>
-      </c>
-      <c r="U3" s="9">
-        <v>1.3888888888888888E-2</v>
-      </c>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="14">
-        <f>SUM(G4:W4)</f>
-        <v>1.2083333333333333</v>
-      </c>
-      <c r="G4" s="9">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="H4" s="9">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="I4" s="9">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="N4" s="9">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="W4" s="9">
-        <v>0.33333333333333331</v>
-      </c>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="F9" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9">
-        <f>SUM(G5:H5)</f>
-        <v>0.3125</v>
-      </c>
-      <c r="G5" s="9">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0.23958333333333334</v>
-      </c>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="J11" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="9"/>
-      <c r="F9" s="8"/>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="10"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="9"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F14" s="9"/>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{A79D2AF2-1227-4D12-A2BF-8956FDB1BD67}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{0AC56A28-223D-471D-B267-9BE5C886E872}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{50021A03-DAAF-4595-AEAD-83022D0C0279}"/>
+    <hyperlink ref="N2" r:id="rId4" xr:uid="{D7E712B2-E62D-4DF3-A431-74035B49EFBE}"/>
+    <hyperlink ref="O2" r:id="rId5" xr:uid="{84D2433F-BC86-4A08-9185-FFE3EB9CD1D8}"/>
+    <hyperlink ref="P2" r:id="rId6" xr:uid="{78E5073F-21E5-4E21-B9FF-C688F1AD0D72}"/>
+    <hyperlink ref="Q2" r:id="rId7" xr:uid="{7A8E866E-211C-4DB2-9261-83085034BF88}"/>
+    <hyperlink ref="R2" r:id="rId8" xr:uid="{B3091946-0451-489D-A2C7-25E196A8194E}"/>
+    <hyperlink ref="S2" r:id="rId9" xr:uid="{F2E1ABE3-647E-4228-9A66-C092175212EB}"/>
+    <hyperlink ref="T2" r:id="rId10" xr:uid="{F1D096EC-6A9B-490D-BA5C-386193558D35}"/>
+    <hyperlink ref="U2" r:id="rId11" xr:uid="{0657B2E3-155A-4BAA-8F70-3EEA1E970BEC}"/>
+    <hyperlink ref="V2" r:id="rId12" xr:uid="{246BA483-75EE-44EF-BD04-550F09CB4980}"/>
+    <hyperlink ref="W2" r:id="rId13" xr:uid="{FDB0044F-13A7-4D68-B05C-100E124285C0}"/>
+    <hyperlink ref="X2" r:id="rId14" xr:uid="{98BB6417-641C-4E91-9FA2-2CA89C5D5F93}"/>
+    <hyperlink ref="Y2" r:id="rId15" xr:uid="{71088EAF-B6B4-4644-B5D1-46B696219A3F}"/>
+    <hyperlink ref="Z2" r:id="rId16" xr:uid="{F0B2CB0C-8605-49C5-BBC5-A261F592033B}"/>
+    <hyperlink ref="K5" r:id="rId17" xr:uid="{B7FEB74C-3C29-445E-9E07-9D8788437723}"/>
+    <hyperlink ref="L5" r:id="rId18" xr:uid="{613308F7-D46E-4E46-8221-FDDAE8344E0E}"/>
+    <hyperlink ref="K4" r:id="rId19" xr:uid="{A0089FA3-7171-446E-BD1A-0D046D81846F}"/>
+    <hyperlink ref="L4" r:id="rId20" xr:uid="{9444324C-0328-4F70-95E4-9DDFBBB4D5DF}"/>
+    <hyperlink ref="M4" r:id="rId21" xr:uid="{2835EBC0-FD03-47C9-9C3A-92B4981B5872}"/>
+    <hyperlink ref="N4" r:id="rId22" xr:uid="{37191584-B0C1-4A49-B0B2-E951AC5366DF}"/>
+    <hyperlink ref="O4" r:id="rId23" xr:uid="{0115A29C-E71B-4534-B0A9-7C73AF067B14}"/>
+    <hyperlink ref="P4" r:id="rId24" xr:uid="{0C3DD7D9-C9AE-43F1-95A3-FF6850CB2B97}"/>
+    <hyperlink ref="Q4" r:id="rId25" xr:uid="{D680FB19-2733-4F5D-BD6E-5A8C4DDD63F6}"/>
+    <hyperlink ref="R4" r:id="rId26" xr:uid="{73566512-ADD4-450D-BBE4-F94744647231}"/>
+    <hyperlink ref="S4" r:id="rId27" xr:uid="{29A3A637-8DED-4090-A256-855623839C6F}"/>
+    <hyperlink ref="K3" r:id="rId28" xr:uid="{79807BB6-6851-40A4-86F8-4978D226D6E1}"/>
+    <hyperlink ref="T3" r:id="rId29" xr:uid="{770BB871-F7D3-47F7-9615-8004E5DCC512}"/>
+    <hyperlink ref="U3" r:id="rId30" xr:uid="{1EAFD715-A6D2-4023-9A9E-31FD41DB47CB}"/>
+    <hyperlink ref="V3" r:id="rId31" xr:uid="{09C2FB7D-9C30-4698-AC3A-41A82C7C76D4}"/>
+    <hyperlink ref="W3" r:id="rId32" xr:uid="{62E3884C-22F5-4A65-8E34-E642BD446A15}"/>
+    <hyperlink ref="X3" r:id="rId33" xr:uid="{0E546202-8972-4F52-AFBC-5690620F6EA2}"/>
+    <hyperlink ref="Y3" r:id="rId34" xr:uid="{CCBDFA6B-0EC0-4AFC-B1AE-CF092D46EA22}"/>
+    <hyperlink ref="L3" r:id="rId35" xr:uid="{501C645C-2F29-4939-BC17-98E843FBC8E5}"/>
+    <hyperlink ref="M3" r:id="rId36" xr:uid="{E4B58205-73BC-4585-BA0D-326E2BD68B1D}"/>
+    <hyperlink ref="N3" r:id="rId37" xr:uid="{6694652D-CC26-410E-9F84-332926BEBBF3}"/>
+    <hyperlink ref="O3" r:id="rId38" xr:uid="{87A21207-F995-4086-890D-3451E0D5A16D}"/>
+    <hyperlink ref="P3" r:id="rId39" xr:uid="{CC5D0EDB-92DF-4235-A01C-36070E7864EA}"/>
+    <hyperlink ref="Q3" r:id="rId40" xr:uid="{342F1333-6903-4C6C-90CA-BB8DD0CCB554}"/>
+    <hyperlink ref="R3" r:id="rId41" xr:uid="{D7300069-3111-4AAF-9F27-829140C02E32}"/>
+    <hyperlink ref="S3" r:id="rId42" xr:uid="{6680142A-8F49-4D05-8B68-D43A41329BC3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>